<commit_message>
added DC/DC converters and changed power source to 24V
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studium_ESE\4. Semester\Ubiquitous Computing Lab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studium_ESE\4. Semester\Ubiquitous Computing Lab\git_repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA4BB01-5ADC-4438-9E8D-3FF899906C97}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4728940-45D5-43D8-9EE4-FB18D6CBEED7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C8A47BDF-107F-4DF2-BFBD-27E994C888F3}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="81">
   <si>
     <t>BOM</t>
   </si>
@@ -248,6 +248,33 @@
   </si>
   <si>
     <t>https://www.amazon.de/dp/B07CQG6CMT/ref=sspa_dk_detail_0?psc=1&amp;pd_rd_i=B07CQG6CMT&amp;pd_rd_w=TFKlj&amp;pf_rd_p=ba8dd0a6-f259-424f-a55c-308aa41eb539&amp;pd_rd_wg=MFl9v&amp;pf_rd_r=QQAFN6WR0YGP7T7THTW7&amp;pd_rd_r=9a6656b2-e960-40d0-ac4e-ee5f33a1b157&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEyM1BIOVVWRE1UTTFHJmVuY3J5cHRlZElkPUEwMzE5Mjg3MzBOU0hCSVVTSTFQRyZlbmNyeXB0ZWRBZElkPUEwNDM2MDQxMUFBVUZQS0hYWE00RiZ3aWRnZXROYW1lPXNwX2RldGFpbCZhY3Rpb249Y2xpY2tSZWRpcmVjdCZkb05vdExvZ0NsaWNrPXRydWU=</t>
+  </si>
+  <si>
+    <t>Buck Converter</t>
+  </si>
+  <si>
+    <t>https://www.conrad.de/de/p/mini-dc-dc-step-down-spannungsregler-mp1584en-buck-power-module-outout-0-8-20v-3a-802244075.html</t>
+  </si>
+  <si>
+    <t>Sonstiges</t>
+  </si>
+  <si>
+    <t>Buck-Converter ESP32</t>
+  </si>
+  <si>
+    <t>24V(Netzteil) --&gt; 12V (Riegel)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DC/DC- Wandler </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DC/DC Converter </t>
+  </si>
+  <si>
+    <t>24V(Netzteil) --&gt; 5V (ESP32)</t>
+  </si>
+  <si>
+    <t>https://www.conrad.de/de/p/dc-dc-9v-12v-24v-to-5v-3a-step-down-voltage-regulator-power-modul-car-charger-802244039.html</t>
   </si>
 </sst>
 </file>
@@ -257,7 +284,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,6 +312,12 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -323,7 +356,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -339,6 +372,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -654,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AFED540-9127-46AD-A742-C9448A4DAE18}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -715,7 +749,7 @@
       <c r="A4" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="15" t="s">
         <v>40</v>
       </c>
       <c r="F4" s="10">
@@ -731,7 +765,7 @@
         <v>41</v>
       </c>
       <c r="F5" s="10">
-        <f t="shared" ref="F5:F40" si="0">D5*E5</f>
+        <f t="shared" ref="F5:F43" si="0">D5*E5</f>
         <v>0</v>
       </c>
     </row>
@@ -832,7 +866,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="15" t="s">
         <v>52</v>
       </c>
     </row>
@@ -844,7 +878,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="15" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1018,200 +1052,262 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B26" s="11"/>
+      <c r="A26" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="10">
+        <v>3</v>
+      </c>
+      <c r="E26" s="10">
+        <v>1</v>
+      </c>
       <c r="F26" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G26" s="11"/>
+        <v>3</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="12" t="s">
-        <v>1</v>
-      </c>
+      <c r="B27" s="11"/>
       <c r="F27" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="G27" s="11"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="F28" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F28" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B29" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D29" s="10">
-        <v>24.5</v>
-      </c>
-      <c r="E29" s="10">
-        <v>1</v>
-      </c>
       <c r="F29" s="10">
         <f t="shared" si="0"/>
-        <v>24.5</v>
-      </c>
-      <c r="G29" s="11" t="s">
-        <v>62</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="10" t="s">
+      <c r="B30" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="10">
+        <v>21.65</v>
+      </c>
+      <c r="E30" s="10">
+        <v>1</v>
+      </c>
+      <c r="F30" s="10">
+        <f t="shared" si="0"/>
+        <v>21.65</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="F30" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F31" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="12" t="s">
+      <c r="F32" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F32" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="10" t="s">
+      <c r="F33" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B34" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C34" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D33" s="10">
+      <c r="D34" s="10">
         <v>2.8</v>
       </c>
-      <c r="E33" s="10">
+      <c r="E34" s="10">
         <v>5</v>
       </c>
-      <c r="F33" s="10">
+      <c r="F34" s="10">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="G33" s="11" t="s">
+      <c r="G34" s="11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B34" s="10" t="s">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B35" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F34" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="10" t="s">
+      <c r="F35" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B36" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E35" s="10">
-        <v>1</v>
-      </c>
-      <c r="F35" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B36" s="10" t="s">
+      <c r="E36" s="10">
+        <v>1</v>
+      </c>
+      <c r="F36" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B37" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F36" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F37" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" s="12" t="s">
+      <c r="F38" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="F38" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" s="10" t="s">
+      <c r="F39" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B40" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C40" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D39" s="10">
+      <c r="D40" s="10">
         <v>9.9499999999999993</v>
       </c>
-      <c r="E39" s="10">
+      <c r="E40" s="10">
         <v>4</v>
       </c>
-      <c r="F39" s="10">
+      <c r="F40" s="10">
         <f t="shared" si="0"/>
         <v>39.799999999999997</v>
       </c>
-      <c r="G39" s="11" t="s">
+      <c r="G40" s="11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="F40" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="10" t="s">
+      <c r="F41" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F42" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D43" s="10">
+        <v>3.45</v>
+      </c>
+      <c r="E43" s="10">
+        <v>2</v>
+      </c>
+      <c r="F43" s="10">
+        <f t="shared" si="0"/>
+        <v>6.9</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G44" s="11"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="F41" s="10">
-        <f>SUM(F3:F40)</f>
-        <v>280.79000000000002</v>
+      <c r="F45" s="12">
+        <f>SUM(F3:F44)</f>
+        <v>287.83999999999997</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G29" r:id="rId1" xr:uid="{474E422B-89CB-48AC-8BB6-4D9F6BF200E4}"/>
-    <hyperlink ref="G33" r:id="rId2" xr:uid="{B35BF1B7-3C72-48A5-8871-D702B7C45E7D}"/>
-    <hyperlink ref="G39" r:id="rId3" xr:uid="{2283879D-93CA-40EA-BB02-555917299B1B}"/>
-    <hyperlink ref="G3" r:id="rId4" display="https://www.amazon.de/GEZE-Rollan-Schiebet%C3%BCrbeschlag-Schiebet%C3%BCr-T%C3%BCrbreite/dp/B000VD8YI6/ref=asc_df_B000VD8YI6/?tag=googshopde-21&amp;linkCode=df0&amp;hvadid=309821455670&amp;hvpos=1o5&amp;hvnetw=g&amp;hvrand=1763377360468305416&amp;hvpone=&amp;hvptwo=&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=9068382&amp;hvtargid=pla-692598411980&amp;psc=1&amp;th=1&amp;psc=1&amp;tag=&amp;ref=&amp;adgrpid=67367133771&amp;hvpone=&amp;hvptwo=&amp;hvadid=309821455670&amp;hvpos=1o5&amp;hvnetw=g&amp;hvrand=1763377360468305416&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=9068382&amp;hvtargid=pla-692598411980" xr:uid="{D49BF5C2-41EF-4DA1-BCCD-BBF7A1AD8F87}"/>
-    <hyperlink ref="G6" r:id="rId5" xr:uid="{45CFB758-23E5-4420-B19C-89088E5F2A34}"/>
-    <hyperlink ref="G9" r:id="rId6" xr:uid="{3AC3DB59-4BE0-4E42-80A4-8A3A37ADBE3B}"/>
-    <hyperlink ref="G12" r:id="rId7" display="https://www.amazon.de/ASHATA-Zahnriemen-3D-Drucker-Riemenscheibe-Synchronriemen-3-Meter/dp/B07PFD7H78/ref=sr_1_21_sspa?__mk_de_DE=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;keywords=zahnriemenscheibe+gt2&amp;qid=1573386082&amp;s=diy&amp;sr=1-21-spons&amp;psc=1&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUExUlJYUlNOSVBRMDI4JmVuY3J5cHRlZElkPUEwMDE1MzAwM0MwQzM5WkFEVE5HNiZlbmNyeXB0ZWRBZElkPUEwNjgxMjM5MzVRR0YzSE1ETTdZTCZ3aWRnZXROYW1lPXNwX2J0ZiZhY3Rpb249Y2xpY2tSZWRpcmVjdCZkb05vdExvZ0NsaWNrPXRydWU=" xr:uid="{E14D096F-5E7C-4E12-9001-20E5460547D1}"/>
-    <hyperlink ref="G17" r:id="rId8" xr:uid="{2DCB2F94-79BD-4949-ACB3-A12463794C56}"/>
-    <hyperlink ref="G21" r:id="rId9" display="https://www.amazon.de/ATOPLEE-T%C3%BCr-Fach-Zunge-Down-Elektroschloss-Montag-Magnet-554239mm/dp/B01N650528/ref=sr_1_21_sspa?__mk_de_DE=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;keywords=t%C3%BCrschloss+elektromagnet&amp;qid=1573743957&amp;sr=8-21-spons&amp;psc=1&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEyMEFKVURJRjdaNU1MJmVuY3J5cHRlZElkPUEwMTc0NjIwMUFDMlJYQTBRRjZYMCZlbmNyeXB0ZWRBZElkPUEwNzY2NDYwMVEzNjdWOFpMQUVYUCZ3aWRnZXROYW1lPXNwX210ZiZhY3Rpb249Y2xpY2tSZWRpcmVjdCZkb05vdExvZ0NsaWNrPXRydWU=" xr:uid="{CDE4F0B4-8F8E-4D2E-B2EF-81644DB8A2F1}"/>
+    <hyperlink ref="G34" r:id="rId1" xr:uid="{B35BF1B7-3C72-48A5-8871-D702B7C45E7D}"/>
+    <hyperlink ref="G40" r:id="rId2" xr:uid="{2283879D-93CA-40EA-BB02-555917299B1B}"/>
+    <hyperlink ref="G3" r:id="rId3" display="https://www.amazon.de/GEZE-Rollan-Schiebet%C3%BCrbeschlag-Schiebet%C3%BCr-T%C3%BCrbreite/dp/B000VD8YI6/ref=asc_df_B000VD8YI6/?tag=googshopde-21&amp;linkCode=df0&amp;hvadid=309821455670&amp;hvpos=1o5&amp;hvnetw=g&amp;hvrand=1763377360468305416&amp;hvpone=&amp;hvptwo=&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=9068382&amp;hvtargid=pla-692598411980&amp;psc=1&amp;th=1&amp;psc=1&amp;tag=&amp;ref=&amp;adgrpid=67367133771&amp;hvpone=&amp;hvptwo=&amp;hvadid=309821455670&amp;hvpos=1o5&amp;hvnetw=g&amp;hvrand=1763377360468305416&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=9068382&amp;hvtargid=pla-692598411980" xr:uid="{D49BF5C2-41EF-4DA1-BCCD-BBF7A1AD8F87}"/>
+    <hyperlink ref="G6" r:id="rId4" xr:uid="{45CFB758-23E5-4420-B19C-89088E5F2A34}"/>
+    <hyperlink ref="G9" r:id="rId5" xr:uid="{3AC3DB59-4BE0-4E42-80A4-8A3A37ADBE3B}"/>
+    <hyperlink ref="G12" r:id="rId6" display="https://www.amazon.de/ASHATA-Zahnriemen-3D-Drucker-Riemenscheibe-Synchronriemen-3-Meter/dp/B07PFD7H78/ref=sr_1_21_sspa?__mk_de_DE=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;keywords=zahnriemenscheibe+gt2&amp;qid=1573386082&amp;s=diy&amp;sr=1-21-spons&amp;psc=1&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUExUlJYUlNOSVBRMDI4JmVuY3J5cHRlZElkPUEwMDE1MzAwM0MwQzM5WkFEVE5HNiZlbmNyeXB0ZWRBZElkPUEwNjgxMjM5MzVRR0YzSE1ETTdZTCZ3aWRnZXROYW1lPXNwX2J0ZiZhY3Rpb249Y2xpY2tSZWRpcmVjdCZkb05vdExvZ0NsaWNrPXRydWU=" xr:uid="{E14D096F-5E7C-4E12-9001-20E5460547D1}"/>
+    <hyperlink ref="G17" r:id="rId7" xr:uid="{2DCB2F94-79BD-4949-ACB3-A12463794C56}"/>
+    <hyperlink ref="G21" r:id="rId8" display="https://www.amazon.de/ATOPLEE-T%C3%BCr-Fach-Zunge-Down-Elektroschloss-Montag-Magnet-554239mm/dp/B01N650528/ref=sr_1_21_sspa?__mk_de_DE=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;keywords=t%C3%BCrschloss+elektromagnet&amp;qid=1573743957&amp;sr=8-21-spons&amp;psc=1&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEyMEFKVURJRjdaNU1MJmVuY3J5cHRlZElkPUEwMTc0NjIwMUFDMlJYQTBRRjZYMCZlbmNyeXB0ZWRBZElkPUEwNzY2NDYwMVEzNjdWOFpMQUVYUCZ3aWRnZXROYW1lPXNwX210ZiZhY3Rpb249Y2xpY2tSZWRpcmVjdCZkb05vdExvZ0NsaWNrPXRydWU=" xr:uid="{CDE4F0B4-8F8E-4D2E-B2EF-81644DB8A2F1}"/>
+    <hyperlink ref="G30" r:id="rId9" xr:uid="{75ADDBAC-F96A-4AF8-ABAC-6D7C807AA2E9}"/>
+    <hyperlink ref="G43" r:id="rId10" xr:uid="{AC7BB9DA-10A4-4663-B041-C7B1F81D0E08}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 
@@ -1219,8 +1315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3A98058-A740-4569-9F16-6D13DE96F8B2}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B20" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>